<commit_message>
data behandling pilot scale
</commit_message>
<xml_diff>
--- a/data/Multisalt/IC_data_multisalt.xlsx
+++ b/data/Multisalt/IC_data_multisalt.xlsx
@@ -10,8 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="917" documentId="8_{FBD22ADF-D34B-44EC-AFF0-58D945556345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C86C86FE-3311-434E-9F86-4F0DD52EE47A}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="1410" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{AC466690-D6AC-4B1F-8149-E6A859686B22}"/>
-    <workbookView xWindow="4920" yWindow="1755" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{7365E4D7-7CF5-48B7-8BD6-1503F6010775}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{7365E4D7-7CF5-48B7-8BD6-1503F6010775}"/>
   </bookViews>
   <sheets>
     <sheet name="Cl" sheetId="1" r:id="rId1"/>
@@ -10026,10 +10025,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C203B86-BC37-486D-A362-C22AA44BAC95}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10848,7 +10846,6 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11666,7 +11663,6 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12485,10 +12481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5A480F-3131-4E1C-9454-44C77B1A1D37}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
-    </sheetView>
-    <sheetView topLeftCell="A22" workbookViewId="1">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
@@ -13343,10 +13336,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAAA244-54FD-4204-9C3F-8E8982A72928}">
   <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A18"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -15347,7 +15339,7 @@
         <v>2.5859999999999999</v>
       </c>
       <c r="D163" s="1">
-        <f t="shared" ref="D162:D176" si="8">(B163+0.0682)/0.2589</f>
+        <f t="shared" ref="D163:D176" si="8">(B163+0.0682)/0.2589</f>
         <v>2.5809192738509075</v>
       </c>
       <c r="E163" s="1"/>

</xml_diff>